<commit_message>
[CODE] init excel reader
</commit_message>
<xml_diff>
--- a/features_files/template/Template_Features.xlsx
+++ b/features_files/template/Template_Features.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
+    <sheet name="Types" sheetId="2" r:id="rId2"/>
+    <sheet name="Features" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -404,22 +406,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="31.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="32.5703125" defaultRowHeight="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="31.5703125" style="1"/>
-    <col min="5" max="5" width="38.42578125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="31.5703125" style="1"/>
-    <col min="8" max="8" width="37.7109375" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="31.5703125" style="1"/>
+    <col min="1" max="16384" width="32.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -431,36 +429,74 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="E2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="32.5703125" defaultRowHeight="72.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="32.5703125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="38.42578125" defaultRowHeight="87.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>